<commit_message>
add protection to the template report
</commit_message>
<xml_diff>
--- a/data-raw/template_report2.xlsx
+++ b/data-raw/template_report2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcuser\OneDrive\IMPROVAST\ACS\CSIemail\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07c4d937b78de3ca/IMPROVAST/ACS/CSIemail/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2350AAC6-AD2B-44FE-85DB-8328938F733E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{2350AAC6-AD2B-44FE-85DB-8328938F733E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AB735E2-08E2-4B2E-81F3-F9A27EDD2690}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -481,6 +481,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -763,7 +767,7 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -5923,32 +5927,32 @@
       <c r="E1000" s="14"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+Oc8lkGb61nADzjFWLbpCUlgPT8yc4STxKB5YcBH4CaR4gQlaRxmMBnbKgqqIbcAQVNdN1OnQVEv7LpmdvbkeQ==" saltValue="g8lE9qngWqLHHmD1SWljnw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="J1:L1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="L3:M1000">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="F3:F1000">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:M1000">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F1000">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>